<commit_message>
upd working fix errors
</commit_message>
<xml_diff>
--- a/SCBAA/2016/BARMM.xlsx
+++ b/SCBAA/2016/BARMM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mngx\thesis\SCBAA\2016\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63BEA277-93BB-4E78-BA93-88056CEE2CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43314F5A-6000-4375-B111-9AB00D468ED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12570" yWindow="345" windowWidth="14880" windowHeight="7260" activeTab="1" xr2:uid="{FCCC59F1-88A9-4466-AAB0-E027C4520B94}"/>
+    <workbookView xWindow="3180" yWindow="1005" windowWidth="14880" windowHeight="11070" xr2:uid="{FCCC59F1-88A9-4466-AAB0-E027C4520B94}"/>
   </bookViews>
   <sheets>
     <sheet name="Isabela" sheetId="1" r:id="rId1"/>
@@ -980,8 +980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39F9E7C8-AAFF-4263-AC86-A6CA2712B14C}">
   <dimension ref="A1:I112"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E109" activeCellId="29" sqref="E10 E15 E20 E23 E28 E32 E41 E45 E49 E53 E57 E61 E65 E69 E73 E74 E77 E80 E83 E86 E89 E94 E95 E97 E99 E101 E103 E105 E107 E109"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1138,7 +1138,6 @@
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="25">
-        <f>SUM(E11:E13)</f>
         <v>0</v>
       </c>
     </row>
@@ -1192,7 +1191,6 @@
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="25">
-        <f>SUM(E16:E18)</f>
         <v>0</v>
       </c>
     </row>
@@ -1383,7 +1381,6 @@
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
       <c r="E37" s="25">
-        <f>SUM(E14,E19,E21:E36)</f>
         <v>439381955.81999999</v>
       </c>
     </row>
@@ -1516,7 +1513,6 @@
         <v>26</v>
       </c>
       <c r="E50" s="37">
-        <f>24506064.18-263813.25</f>
         <v>24242250.93</v>
       </c>
     </row>
@@ -1812,7 +1808,6 @@
         <v>14</v>
       </c>
       <c r="E78" s="37">
-        <f>9030468+5000000</f>
         <v>14030468</v>
       </c>
       <c r="F78" s="19"/>
@@ -1951,7 +1946,6 @@
         <v>14</v>
       </c>
       <c r="E91" s="37">
-        <f>17272822.5+28305705.15</f>
         <v>45578527.649999999</v>
       </c>
     </row>
@@ -1972,7 +1966,6 @@
       </c>
       <c r="D93" s="8"/>
       <c r="E93" s="17">
-        <f>SUM(E41:E92)</f>
         <v>457992881.74999994</v>
       </c>
     </row>
@@ -2148,7 +2141,6 @@
         <v>1</v>
       </c>
       <c r="E111" s="4">
-        <f>SUM(E96,E98,E100,E102,E104,E106,E108,E110)</f>
         <v>0</v>
       </c>
     </row>
@@ -2160,7 +2152,6 @@
       <c r="C112" s="2"/>
       <c r="D112" s="2"/>
       <c r="E112" s="1">
-        <f>SUM(E93,E111)</f>
         <v>457992881.74999994</v>
       </c>
     </row>
@@ -2182,7 +2173,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9EF0239-B27D-4590-8540-2F5B458C0B15}">
   <dimension ref="A1:P112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>

</xml_diff>